<commit_message>
fix reset with events
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="440" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="440" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
   <si>
     <t>Events</t>
   </si>
@@ -41,13 +41,13 @@
     <t>Key (Case Insensitive)</t>
   </si>
   <si>
+    <t>Gnome</t>
+  </si>
+  <si>
     <t>Song Genre</t>
   </si>
   <si>
     <t>Specifications</t>
-  </si>
-  <si>
-    <t>Creepy</t>
   </si>
   <si>
     <t xml:space="preserve">(∩ ͡° ͜ʖ ͡°)⊃━☆ﾟ. * ･ ｡ </t>
@@ -226,9 +226,6 @@
     <t>For example, for a 3-lane highway, each block is 4 columns wide.</t>
   </si>
   <si>
-    <t>TO ADD LATER: specify regions of the document and how many to select from each region</t>
-  </si>
-  <si>
     <t>Padding between enemies:</t>
   </si>
   <si>
@@ -371,23 +368,26 @@
     <t>bensound-funkyelement.mp3</t>
   </si>
   <si>
-    <t>bensound-ofeliasdream.mp3</t>
-  </si>
-  <si>
     <t>bensound-countryboy.mp3</t>
   </si>
   <si>
     <t>Less</t>
   </si>
   <si>
-    <t>Rear enemy</t>
+    <t>Rear Enemy</t>
+  </si>
+  <si>
+    <t>Ned wakes up</t>
+  </si>
+  <si>
+    <t>Nosh wakes up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -439,13 +439,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="13"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Body)"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="13"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -453,7 +452,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -486,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -503,12 +507,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -805,7 +810,7 @@
     <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -816,7 +821,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -831,9 +836,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>25</v>
@@ -842,16 +847,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -859,13 +861,16 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -873,40 +878,55 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D5" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J5" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="E6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="15"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="12"/>
+      <c r="K7" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J9" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -915,98 +935,129 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="K11" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J13" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="E14" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="K15" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I16" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J17" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" ht="26" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+      <c r="E18" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="K19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1014,15 +1065,18 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G25" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1033,38 +1087,38 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1072,7 +1126,7 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -1081,16 +1135,16 @@
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
-        <v>50</v>
+      <c r="A33" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
-        <v>51</v>
+      <c r="A34" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
@@ -1098,7 +1152,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
@@ -1106,7 +1160,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
@@ -1114,7 +1168,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
@@ -1122,7 +1176,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
@@ -1168,7 +1222,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>

</xml_diff>

<commit_message>
fixed the radio thing
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="320" yWindow="440" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="440" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -794,7 +794,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:H24"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
sun in the test level and fixed eventhandler pop
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stsinwell/cs/MangoSnoopers/core/assets/levels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E046F6B1-2A60-4B17-977E-3E0FC3F04DC9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="440" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
+    <workbookView xWindow="1875" yWindow="435" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
   <si>
     <t>Events</t>
   </si>
@@ -381,13 +382,19 @@
   </si>
   <si>
     <t>Nosh wakes up</t>
+  </si>
+  <si>
+    <t>Sun start</t>
+  </si>
+  <si>
+    <t>Sun end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -523,6 +530,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -790,27 +800,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -836,7 +846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -850,10 +860,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -870,7 +880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -887,10 +897,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
         <v>16</v>
       </c>
@@ -902,7 +915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -914,7 +927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -926,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -934,8 +947,11 @@
         <v>55</v>
       </c>
       <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E10" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -947,7 +963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="D12" s="6"/>
       <c r="E12" s="2" t="s">
         <v>59</v>
@@ -956,13 +972,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="D13" s="6"/>
       <c r="G13" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -971,7 +987,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -980,7 +996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -989,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -998,7 +1014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -1007,7 +1023,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="21">
       <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
@@ -1018,13 +1034,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1032,7 +1048,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -1040,7 +1056,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
@@ -1054,7 +1070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1062,7 +1078,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -1073,7 +1089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1084,7 +1100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1093,7 +1109,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="8" t="s">
         <v>43</v>
       </c>
@@ -1101,13 +1117,13 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" s="6" customFormat="1">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
@@ -1115,7 +1131,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1123,7 +1139,7 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -1131,7 +1147,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="13" t="s">
         <v>49</v>
       </c>
@@ -1139,7 +1155,7 @@
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -1147,7 +1163,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" s="5" t="s">
         <v>44</v>
       </c>
@@ -1155,7 +1171,7 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" s="5" t="s">
         <v>45</v>
       </c>
@@ -1163,7 +1179,7 @@
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="5" t="s">
         <v>46</v>
       </c>
@@ -1171,7 +1187,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -1179,13 +1195,13 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -1193,7 +1209,7 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
@@ -1201,7 +1217,7 @@
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
@@ -1209,7 +1225,7 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="4" t="s">
         <v>28</v>
       </c>
@@ -1217,7 +1233,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
         <v>37</v>
       </c>
@@ -1225,13 +1241,13 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
         <v>29</v>
       </c>
@@ -1239,7 +1255,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -1247,7 +1263,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="5" t="s">
         <v>31</v>
       </c>
@@ -1255,7 +1271,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="5" t="s">
         <v>32</v>
       </c>
@@ -1263,7 +1279,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="4" t="s">
         <v>33</v>
       </c>
@@ -1271,13 +1287,13 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="10" t="s">
         <v>19</v>
       </c>
@@ -1285,7 +1301,7 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="4" t="s">
         <v>22</v>
       </c>
@@ -1293,7 +1309,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="4" t="s">
         <v>23</v>
       </c>
@@ -1301,13 +1317,13 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>

</xml_diff>

<commit_message>
there was a bug to my bug fix go figure
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E046F6B1-2A60-4B17-977E-3E0FC3F04DC9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FBC4F3-A5AD-4912-A1E4-A43679411081}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="435" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="435" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -804,7 +804,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>
@@ -947,9 +947,6 @@
         <v>55</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="2" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
@@ -1001,6 +998,9 @@
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
+      <c r="E16" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="F16" s="12" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
DID WE FIX IT ?? WHAT'S GOING ON
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FBC4F3-A5AD-4912-A1E4-A43679411081}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18FFDC1-EB33-4D22-AD9E-24ABD3F2A8A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="435" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="435" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -804,7 +804,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F4" sqref="F4:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>

</xml_diff>

<commit_message>
bfig video -- master branch plus some stuff from sterlock for rest stops
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stsinwell/cs/MangoSnoopers/core/assets/levels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B18FFDC1-EB33-4D22-AD9E-24ABD3F2A8A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="435" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3740" yWindow="440" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>Events</t>
   </si>
@@ -372,16 +371,7 @@
     <t>bensound-countryboy.mp3</t>
   </si>
   <si>
-    <t>Less</t>
-  </si>
-  <si>
     <t>Rear Enemy</t>
-  </si>
-  <si>
-    <t>Ned wakes up</t>
-  </si>
-  <si>
-    <t>Nosh wakes up</t>
   </si>
   <si>
     <t>Sun start</t>
@@ -393,8 +383,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -800,27 +790,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:H26"/>
+      <selection activeCell="G44" sqref="G41:H44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="2"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -846,7 +836,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -860,10 +850,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -880,7 +870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -888,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="D5" s="11">
         <v>0</v>
@@ -897,25 +887,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D6" s="6"/>
-      <c r="E6" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="16"/>
-      <c r="E7" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="H7" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -923,11 +907,9 @@
         <v>10</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="F8" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -935,11 +917,12 @@
         <v>54</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="G9" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="F9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -948,7 +931,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -956,35 +939,28 @@
         <v>56</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="H11" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="6"/>
-      <c r="E12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D13" s="6"/>
+      <c r="E13" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="G13" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -993,37 +969,34 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="F16" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
+      <c r="E17" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="G17" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="21">
+    </row>
+    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
@@ -1034,13 +1007,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="F20" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1048,29 +1024,26 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="G22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="F23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1078,29 +1051,32 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="G25" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="F25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="E26" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1109,7 +1085,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>43</v>
       </c>
@@ -1117,13 +1093,19 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" s="6" customFormat="1">
+      <c r="F29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
@@ -1131,15 +1113,18 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="H31" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -1147,15 +1132,18 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="G33" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -1163,7 +1151,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>44</v>
       </c>
@@ -1171,15 +1159,18 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="F36" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>46</v>
       </c>
@@ -1187,7 +1178,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -1195,13 +1186,13 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -1209,15 +1200,18 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
@@ -1225,7 +1219,7 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>28</v>
       </c>
@@ -1233,21 +1227,25 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>29</v>
       </c>
@@ -1255,7 +1253,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -1263,7 +1261,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>31</v>
       </c>
@@ -1271,7 +1269,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>32</v>
       </c>
@@ -1279,7 +1277,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>33</v>
       </c>
@@ -1287,13 +1285,13 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>19</v>
       </c>
@@ -1301,7 +1299,7 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>22</v>
       </c>
@@ -1309,7 +1307,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>23</v>
       </c>
@@ -1317,13 +1315,13 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>

</xml_diff>

<commit_message>
sat question in duh works
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stsinwell/cs/MangoSnoopers/core/assets/levels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C0D4EE-EFC8-411B-9E15-0E097467E31D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="440" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
+    <workbookView xWindow="4695" yWindow="435" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>Events</t>
   </si>
@@ -378,13 +379,16 @@
   </si>
   <si>
     <t>Sun end</t>
+  </si>
+  <si>
+    <t>SAT Question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -790,27 +794,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G44" sqref="G41:H44"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -836,7 +840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -850,10 +854,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -866,11 +870,14 @@
       <c r="D4" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="F4" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -887,10 +894,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="16" t="s">
         <v>16</v>
       </c>
@@ -899,7 +906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -909,7 +916,7 @@
       <c r="D8" s="6"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -922,7 +929,7 @@
       </c>
       <c r="G9" s="12"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -931,7 +938,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -941,11 +948,11 @@
       <c r="D11" s="6"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="D12" s="6"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="D13" s="6"/>
       <c r="E13" s="2" t="s">
         <v>57</v>
@@ -954,13 +961,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -969,7 +976,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -978,7 +985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -990,13 +997,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="21">
       <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
@@ -1007,7 +1014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -1016,7 +1023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1024,7 +1031,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -1035,7 +1042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
@@ -1043,7 +1050,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1051,7 +1058,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -1065,7 +1072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1076,7 +1083,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1085,7 +1092,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="8" t="s">
         <v>43</v>
       </c>
@@ -1093,7 +1100,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1105,7 +1112,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" s="6" customFormat="1">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
@@ -1113,7 +1120,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1124,7 +1131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -1132,7 +1139,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="13" t="s">
         <v>49</v>
       </c>
@@ -1143,7 +1150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -1151,7 +1158,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
         <v>44</v>
       </c>
@@ -1159,7 +1166,7 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
         <v>45</v>
       </c>
@@ -1170,7 +1177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>46</v>
       </c>
@@ -1178,7 +1185,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -1186,13 +1193,13 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -1200,7 +1207,7 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
@@ -1211,7 +1218,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
@@ -1219,7 +1226,7 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="4" t="s">
         <v>28</v>
       </c>
@@ -1227,7 +1234,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="4" t="s">
         <v>37</v>
       </c>
@@ -1239,13 +1246,13 @@
       </c>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="4" t="s">
         <v>29</v>
       </c>
@@ -1253,7 +1260,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -1261,7 +1268,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>31</v>
       </c>
@@ -1269,7 +1276,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="5" t="s">
         <v>32</v>
       </c>
@@ -1277,7 +1284,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="4" t="s">
         <v>33</v>
       </c>
@@ -1285,13 +1292,13 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="10" t="s">
         <v>19</v>
       </c>
@@ -1299,7 +1306,7 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="4" t="s">
         <v>22</v>
       </c>
@@ -1307,7 +1314,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="4" t="s">
         <v>23</v>
       </c>
@@ -1315,13 +1322,13 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>

</xml_diff>

<commit_message>
multilevel support idk what im doing anymore
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -797,7 +797,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -852,12 +852,12 @@
       <c r="D2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" s="6"/>
+      <c r="G3" s="12" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -887,8 +887,8 @@
       <c r="D5" s="11">
         <v>0</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>4</v>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
quick fix for game crashing at last level
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="440" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
+    <workbookView xWindow="4840" yWindow="660" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Events</t>
   </si>
@@ -371,23 +371,23 @@
     <t>bensound-countryboy.mp3</t>
   </si>
   <si>
+    <t>SAT Question</t>
+  </si>
+  <si>
+    <t>Sun Start</t>
+  </si>
+  <si>
     <t>Rear Enemy</t>
   </si>
   <si>
-    <t>Sun start</t>
-  </si>
-  <si>
-    <t>Sun end</t>
-  </si>
-  <si>
-    <t>SAT Question</t>
+    <t>Sun End</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -463,6 +463,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -490,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -511,6 +518,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -797,7 +805,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -826,16 +834,16 @@
       <c r="D1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="16" t="s">
         <v>14</v>
       </c>
     </row>
@@ -852,12 +860,21 @@
       <c r="D2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2" s="12" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" s="6"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -872,10 +889,12 @@
       <c r="D4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4" s="12"/>
+      <c r="H4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -892,21 +911,31 @@
       <c r="D5" s="11">
         <v>0</v>
       </c>
+      <c r="E5"/>
+      <c r="F5"/>
       <c r="G5" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="H5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D6" s="6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="H7" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="B7" s="17"/>
+      <c r="E7"/>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -916,7 +945,12 @@
         <v>10</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="F8" s="12"/>
+      <c r="E8"/>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -926,10 +960,14 @@
         <v>54</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="F9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="12"/>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -939,6 +977,12 @@
         <v>55</v>
       </c>
       <c r="D10" s="6"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -948,62 +992,88 @@
         <v>56</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="H11" s="12"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="6"/>
-      <c r="F12" s="12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D13" s="6"/>
-      <c r="E13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="H15" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="F16" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16" s="12"/>
+      <c r="H16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="E17"/>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17"/>
+      <c r="H17"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
+      <c r="E18"/>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18"/>
     </row>
     <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
@@ -1012,18 +1082,24 @@
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="H19" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="F20" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
@@ -1032,6 +1108,12 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -1040,7 +1122,10 @@
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="G22" s="2" t="s">
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1051,6 +1136,12 @@
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
@@ -1059,6 +1150,12 @@
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
@@ -1067,12 +1164,12 @@
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="F25" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
@@ -1081,9 +1178,12 @@
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="E26" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
@@ -1092,7 +1192,10 @@
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="1"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
@@ -1107,12 +1210,8 @@
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="F29" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
@@ -1129,9 +1228,7 @@
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="H31" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="H31" s="12"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
@@ -1148,9 +1245,7 @@
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="G33" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="G33" s="12"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
@@ -1175,9 +1270,7 @@
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="F36" s="12" t="s">
-        <v>4</v>
-      </c>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
@@ -1216,9 +1309,6 @@
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">

</xml_diff>

<commit_message>
SAT question bug fix and fullscreen fun
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stsinwell/cs/MangoSnoopers/core/assets/levels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F20A59-18F6-471A-B7B2-1AD5741A0D5C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="660" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
+    <workbookView xWindow="5850" yWindow="660" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>Events</t>
   </si>
@@ -386,8 +387,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -801,27 +802,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -847,7 +848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -867,7 +868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="D3" s="6"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -876,7 +877,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -898,7 +899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -918,14 +919,14 @@
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="D6" s="6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="17" t="s">
         <v>16</v>
       </c>
@@ -937,7 +938,7 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -952,7 +953,7 @@
       <c r="G8" s="12"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -969,7 +970,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -984,7 +985,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -997,7 +998,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="D12" s="6"/>
       <c r="E12"/>
       <c r="F12"/>
@@ -1006,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="D13" s="6"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -1015,7 +1016,7 @@
       </c>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -1029,7 +1030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -1041,7 +1042,7 @@
       </c>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -1051,7 +1052,7 @@
       <c r="G16" s="12"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -1063,7 +1064,7 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -1075,21 +1076,23 @@
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="21">
       <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19"/>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
       <c r="F19"/>
       <c r="G19" t="s">
         <v>4</v>
       </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -1101,7 +1104,7 @@
       </c>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1115,7 +1118,7 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
@@ -1143,7 +1146,7 @@
       </c>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -1171,7 +1174,7 @@
       </c>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1185,7 +1188,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1197,7 +1200,7 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="8" t="s">
         <v>43</v>
       </c>
@@ -1205,7 +1208,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1213,7 +1216,7 @@
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" s="6" customFormat="1">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +1224,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1230,7 +1233,7 @@
       <c r="D31" s="5"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -1238,7 +1241,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="13" t="s">
         <v>49</v>
       </c>
@@ -1247,7 +1250,7 @@
       <c r="D33" s="5"/>
       <c r="G33" s="12"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -1255,7 +1258,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
         <v>44</v>
       </c>
@@ -1263,7 +1266,7 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
         <v>45</v>
       </c>
@@ -1272,7 +1275,7 @@
       <c r="D36" s="5"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>46</v>
       </c>
@@ -1280,7 +1283,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -1288,13 +1291,13 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -1302,7 +1305,7 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
@@ -1310,7 +1313,7 @@
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
@@ -1318,7 +1321,7 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="4" t="s">
         <v>28</v>
       </c>
@@ -1326,7 +1329,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="4" t="s">
         <v>37</v>
       </c>
@@ -1335,13 +1338,13 @@
       <c r="D44" s="5"/>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="4" t="s">
         <v>29</v>
       </c>
@@ -1349,7 +1352,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -1357,7 +1360,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>31</v>
       </c>
@@ -1365,7 +1368,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="5" t="s">
         <v>32</v>
       </c>
@@ -1373,7 +1376,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="4" t="s">
         <v>33</v>
       </c>
@@ -1381,13 +1384,13 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="10" t="s">
         <v>19</v>
       </c>
@@ -1395,7 +1398,7 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="4" t="s">
         <v>22</v>
       </c>
@@ -1403,7 +1406,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="4" t="s">
         <v>23</v>
       </c>
@@ -1411,13 +1414,13 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>

</xml_diff>

<commit_message>
fixed levels that I screwed up
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ted/Documents/Repos/MangoSnoopers/core/assets/levels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F20A59-18F6-471A-B7B2-1AD5741A0D5C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24720" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="5850" yWindow="660" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>Events</t>
   </si>
@@ -39,6 +40,9 @@
   </si>
   <si>
     <t>Key (Case Insensitive)</t>
+  </si>
+  <si>
+    <t>Gnome</t>
   </si>
   <si>
     <t>Song Genre</t>
@@ -378,16 +382,13 @@
   </si>
   <si>
     <t>Sun End</t>
-  </si>
-  <si>
-    <t>Flamingo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -801,104 +802,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>11</v>
-      </c>
       <c r="H1" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3">
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="D3" s="6"/>
       <c r="E3"/>
       <c r="F3"/>
-      <c r="G3" s="12"/>
+      <c r="G3" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4" s="12"/>
       <c r="H4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -906,80 +907,90 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="11">
         <v>0</v>
       </c>
       <c r="E5"/>
       <c r="F5"/>
-      <c r="G5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="D6" s="6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="17"/>
       <c r="E7"/>
-      <c r="F7"/>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8"/>
-      <c r="F8"/>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
       <c r="G8" s="12"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F9"/>
-      <c r="G9" s="12"/>
+      <c r="G9" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10"/>
       <c r="F10"/>
-      <c r="G10"/>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11"/>
@@ -987,43 +998,51 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="D12" s="6"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12" s="12"/>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="D13" s="6"/>
       <c r="E13"/>
       <c r="F13"/>
-      <c r="G13"/>
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15"/>
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -1033,48 +1052,59 @@
       <c r="G16" s="12"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17"/>
-      <c r="F17"/>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18"/>
-      <c r="F18"/>
+      <c r="F18" t="s">
+        <v>4</v>
+      </c>
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="21">
       <c r="A19" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F19"/>
-      <c r="G19"/>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F20"/>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1082,15 +1112,15 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
@@ -1098,23 +1128,27 @@
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
-      <c r="H22"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23"/>
       <c r="F23"/>
-      <c r="G23"/>
+      <c r="G23" t="s">
+        <v>4</v>
+      </c>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
@@ -1122,37 +1156,41 @@
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24"/>
-      <c r="H24"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25"/>
       <c r="F25"/>
-      <c r="G25"/>
+      <c r="G25" t="s">
+        <v>4</v>
+      </c>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
@@ -1162,15 +1200,15 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1178,211 +1216,211 @@
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" s="6" customFormat="1">
       <c r="A30" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="G33" s="12"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>

</xml_diff>

<commit_message>
item indicators, limitations to how many you can take
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stsinwell/cs/MangoSnoopers/core/assets/levels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F20A59-18F6-471A-B7B2-1AD5741A0D5C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5850" yWindow="660" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5860" yWindow="660" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Events</t>
   </si>
@@ -387,8 +386,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -802,27 +801,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="2"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -848,7 +847,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -861,14 +860,14 @@
       <c r="D2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E2"/>
+      <c r="E2" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="F2"/>
       <c r="G2"/>
-      <c r="H2" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" s="6"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -877,7 +876,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -899,7 +898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -919,14 +918,14 @@
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D6" s="6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>16</v>
       </c>
@@ -938,7 +937,7 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -953,7 +952,7 @@
       <c r="G8" s="12"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -970,7 +969,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -985,7 +984,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -998,7 +997,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="6"/>
       <c r="E12"/>
       <c r="F12"/>
@@ -1007,7 +1006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D13" s="6"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -1016,7 +1015,7 @@
       </c>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -1030,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -1042,7 +1041,7 @@
       </c>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -1052,7 +1051,7 @@
       <c r="G16" s="12"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -1064,7 +1063,7 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -1076,7 +1075,7 @@
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" ht="21">
+    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
@@ -1092,7 +1091,7 @@
       </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -1104,7 +1103,7 @@
       </c>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1118,7 +1117,7 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -1132,7 +1131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
@@ -1146,7 +1145,7 @@
       </c>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1160,7 +1159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -1174,21 +1173,18 @@
       </c>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="16" t="s">
-        <v>11</v>
-      </c>
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1200,7 +1196,7 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>43</v>
       </c>
@@ -1208,7 +1204,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1216,7 +1212,7 @@
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1">
+    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
@@ -1224,7 +1220,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1233,7 +1229,7 @@
       <c r="D31" s="5"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -1241,7 +1237,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>49</v>
       </c>
@@ -1250,7 +1246,7 @@
       <c r="D33" s="5"/>
       <c r="G33" s="12"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -1258,7 +1254,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>44</v>
       </c>
@@ -1266,7 +1262,7 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>45</v>
       </c>
@@ -1275,7 +1271,7 @@
       <c r="D36" s="5"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>46</v>
       </c>
@@ -1283,7 +1279,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -1291,13 +1287,13 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -1305,7 +1301,7 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
@@ -1313,7 +1309,7 @@
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
@@ -1321,7 +1317,7 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>28</v>
       </c>
@@ -1329,7 +1325,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>37</v>
       </c>
@@ -1338,13 +1334,13 @@
       <c r="D44" s="5"/>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>29</v>
       </c>
@@ -1352,7 +1348,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -1360,7 +1356,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>31</v>
       </c>
@@ -1368,7 +1364,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>32</v>
       </c>
@@ -1376,7 +1372,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>33</v>
       </c>
@@ -1384,13 +1380,13 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>19</v>
       </c>
@@ -1398,7 +1394,7 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>22</v>
       </c>
@@ -1406,7 +1402,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>23</v>
       </c>
@@ -1414,13 +1410,13 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>

</xml_diff>

<commit_message>
Revert "more touchscreen progress"
This reverts commit 0d4a2554079e8771795eed54cbaf2ad9b9b1efc7.
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stsinwell/cs/MangoSnoopers/core/assets/levels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA172A7-A0BC-4F44-A235-B1CDF65E3C4C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="660" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5860" yWindow="660" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,8 +386,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -802,27 +801,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.875" style="2"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -848,7 +847,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -861,12 +860,14 @@
       <c r="D2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" s="6"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -875,7 +876,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -897,7 +898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -917,14 +918,14 @@
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D6" s="6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>16</v>
       </c>
@@ -936,7 +937,7 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -951,7 +952,7 @@
       <c r="G8" s="12"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -968,7 +969,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -983,7 +984,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -996,7 +997,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="6"/>
       <c r="E12"/>
       <c r="F12"/>
@@ -1005,7 +1006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D13" s="6"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -1014,7 +1015,7 @@
       </c>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -1028,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -1040,7 +1041,7 @@
       </c>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -1050,7 +1051,7 @@
       <c r="G16" s="12"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -1062,7 +1063,7 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -1074,7 +1075,7 @@
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" ht="21">
+    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
@@ -1090,7 +1091,7 @@
       </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -1102,7 +1103,7 @@
       </c>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1116,7 +1117,7 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
@@ -1144,7 +1145,7 @@
       </c>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -1172,7 +1173,7 @@
       </c>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1183,7 +1184,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1195,18 +1196,15 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1214,7 +1212,7 @@
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1">
+    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
@@ -1222,7 +1220,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1231,7 +1229,7 @@
       <c r="D31" s="5"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -1239,7 +1237,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>49</v>
       </c>
@@ -1248,7 +1246,7 @@
       <c r="D33" s="5"/>
       <c r="G33" s="12"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -1256,7 +1254,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>44</v>
       </c>
@@ -1264,7 +1262,7 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>45</v>
       </c>
@@ -1273,7 +1271,7 @@
       <c r="D36" s="5"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>46</v>
       </c>
@@ -1281,7 +1279,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -1289,13 +1287,13 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -1303,7 +1301,7 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
@@ -1311,7 +1309,7 @@
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
@@ -1319,7 +1317,7 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>28</v>
       </c>
@@ -1327,7 +1325,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>37</v>
       </c>
@@ -1336,13 +1334,13 @@
       <c r="D44" s="5"/>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>29</v>
       </c>
@@ -1350,7 +1348,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -1358,7 +1356,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>31</v>
       </c>
@@ -1366,7 +1364,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>32</v>
       </c>
@@ -1374,7 +1372,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>33</v>
       </c>
@@ -1382,13 +1380,13 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>19</v>
       </c>
@@ -1396,7 +1394,7 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>22</v>
       </c>
@@ -1404,7 +1402,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>23</v>
       </c>
@@ -1412,13 +1410,13 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>

</xml_diff>

<commit_message>
been in rhodes for 10 hours
</commit_message>
<xml_diff>
--- a/core/assets/levels/test_level0.xlsx
+++ b/core/assets/levels/test_level0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stsinwell/cs/MangoSnoopers/core/assets/levels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Git\MangoSnoopers\core\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA172A7-A0BC-4F44-A235-B1CDF65E3C4C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="660" windowWidth="29460" windowHeight="22300" tabRatio="500"/>
+    <workbookView xWindow="6870" yWindow="660" windowWidth="29460" windowHeight="22305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,8 +387,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -801,27 +802,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -847,7 +848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -860,14 +861,12 @@
       <c r="D2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>11</v>
-      </c>
+      <c r="E2" s="16"/>
       <c r="F2"/>
       <c r="G2"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="D3" s="6"/>
       <c r="E3"/>
       <c r="F3"/>
@@ -876,7 +875,7 @@
       </c>
       <c r="H3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -898,7 +897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -918,14 +917,14 @@
       </c>
       <c r="H5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="D6" s="6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="17" t="s">
         <v>16</v>
       </c>
@@ -937,7 +936,7 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -952,7 +951,7 @@
       <c r="G8" s="12"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>52</v>
       </c>
@@ -969,7 +968,7 @@
       </c>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -984,7 +983,7 @@
       </c>
       <c r="H10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
@@ -997,7 +996,7 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="D12" s="6"/>
       <c r="E12"/>
       <c r="F12"/>
@@ -1006,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="D13" s="6"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -1015,7 +1014,7 @@
       </c>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -1029,7 +1028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -1041,7 +1040,7 @@
       </c>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -1051,7 +1050,7 @@
       <c r="G16" s="12"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -1063,7 +1062,7 @@
       <c r="G17"/>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -1075,7 +1074,7 @@
       <c r="G18"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="21">
       <c r="A19" s="15" t="s">
         <v>7</v>
       </c>
@@ -1091,7 +1090,7 @@
       </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -1103,7 +1102,7 @@
       </c>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1117,7 +1116,7 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
@@ -1131,7 +1130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="8" t="s">
         <v>24</v>
       </c>
@@ -1145,7 +1144,7 @@
       </c>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="5" t="s">
         <v>38</v>
       </c>
@@ -1173,7 +1172,7 @@
       </c>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="5" t="s">
         <v>9</v>
       </c>
@@ -1184,7 +1183,7 @@
       <c r="G26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="8" t="s">
         <v>36</v>
       </c>
@@ -1196,15 +1195,18 @@
       <c r="G27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E28" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1212,7 +1214,7 @@
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
     </row>
-    <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" s="6" customFormat="1">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
@@ -1220,7 +1222,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="5" t="s">
         <v>21</v>
       </c>
@@ -1229,7 +1231,7 @@
       <c r="D31" s="5"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
@@ -1237,7 +1239,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="13" t="s">
         <v>49</v>
       </c>
@@ -1246,7 +1248,7 @@
       <c r="D33" s="5"/>
       <c r="G33" s="12"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -1254,7 +1256,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="5" t="s">
         <v>44</v>
       </c>
@@ -1262,7 +1264,7 @@
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="5" t="s">
         <v>45</v>
       </c>
@@ -1271,7 +1273,7 @@
       <c r="D36" s="5"/>
       <c r="F36" s="12"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="5" t="s">
         <v>46</v>
       </c>
@@ -1279,7 +1281,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -1287,13 +1289,13 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="9"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
@@ -1301,7 +1303,7 @@
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="4" t="s">
         <v>27</v>
       </c>
@@ -1309,7 +1311,7 @@
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
@@ -1317,7 +1319,7 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" s="4" t="s">
         <v>28</v>
       </c>
@@ -1325,7 +1327,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" s="4" t="s">
         <v>37</v>
       </c>
@@ -1334,13 +1336,13 @@
       <c r="D44" s="5"/>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" s="4" t="s">
         <v>29</v>
       </c>
@@ -1348,7 +1350,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" s="5" t="s">
         <v>30</v>
       </c>
@@ -1356,7 +1358,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="5" t="s">
         <v>31</v>
       </c>
@@ -1364,7 +1366,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="5" t="s">
         <v>32</v>
       </c>
@@ -1372,7 +1374,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="4" t="s">
         <v>33</v>
       </c>
@@ -1380,13 +1382,13 @@
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="4"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="10" t="s">
         <v>19</v>
       </c>
@@ -1394,7 +1396,7 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="4" t="s">
         <v>22</v>
       </c>
@@ -1402,7 +1404,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="4" t="s">
         <v>23</v>
       </c>
@@ -1410,13 +1412,13 @@
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>

</xml_diff>